<commit_message>
Update 9. Ferramentas de Dados
Finalizando módulo. Anotações e Prática. Aulas da 18 à 23.
</commit_message>
<xml_diff>
--- a/9. Ferramentas de Dados/Ferramentas de Dados - Validação de Dados.xlsx
+++ b/9. Ferramentas de Dados/Ferramentas de Dados - Validação de Dados.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kiko\Documents\Projetos Programação\Especializacao-em-Analise-de-Dados\9. Ferramentas de Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8523359E-267D-4612-904E-4F727D940B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A75BFE-B786-4D5E-9250-EC1672E9C888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" tabRatio="538" activeTab="2" xr2:uid="{0D445F65-54A1-41E5-865A-2279466CCF1F}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" tabRatio="538" firstSheet="3" activeTab="4" xr2:uid="{0D445F65-54A1-41E5-865A-2279466CCF1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="2" r:id="rId1"/>
     <sheet name="Paises" sheetId="3" r:id="rId2"/>
     <sheet name="Pratica" sheetId="4" r:id="rId3"/>
+    <sheet name="Planilha1" sheetId="5" r:id="rId4"/>
+    <sheet name="Planilha2" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Paises!$A$1:$E$55</definedName>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="89">
   <si>
     <t>Nome</t>
   </si>
@@ -266,16 +268,63 @@
   </si>
   <si>
     <t>Espanha</t>
+  </si>
+  <si>
+    <t>Mega-Blac</t>
+  </si>
+  <si>
+    <t>Valor Disponível</t>
+  </si>
+  <si>
+    <t>Funcionários</t>
+  </si>
+  <si>
+    <t>Marcus</t>
+  </si>
+  <si>
+    <t>Ana Maria</t>
+  </si>
+  <si>
+    <t>Cláudio</t>
+  </si>
+  <si>
+    <t>Jeferson</t>
+  </si>
+  <si>
+    <t>João</t>
+  </si>
+  <si>
+    <t>Marcela</t>
+  </si>
+  <si>
+    <t>Paula</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Rafaela</t>
+  </si>
+  <si>
+    <t>Alon</t>
+  </si>
+  <si>
+    <t>Priscila</t>
+  </si>
+  <si>
+    <t>Rafael</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="166" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,8 +339,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,6 +392,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -452,10 +528,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -474,8 +551,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
@@ -600,6 +690,50 @@
       </fill>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -608,15 +742,132 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <bottom/>
         <vertical/>
         <horizontal/>
       </border>
@@ -630,22 +881,30 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -685,175 +944,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -868,25 +958,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{94D6C4E3-EC2B-4BCA-A9B6-A7CEE2489B34}" name="Tabela1" displayName="Tabela1" ref="A1:F3" totalsRowShown="0" headerRowDxfId="10" dataDxfId="11" headerRowBorderDxfId="19" tableBorderDxfId="20" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{94D6C4E3-EC2B-4BCA-A9B6-A7CEE2489B34}" name="Tabela1" displayName="Tabela1" ref="A1:F3" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="A1:F3" xr:uid="{94D6C4E3-EC2B-4BCA-A9B6-A7CEE2489B34}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F4433FC6-D4E6-4D1F-98D4-77E7D1A887BA}" name="Nome" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{D5A6E3E8-91CB-4D68-9A74-D97F4D65094A}" name="Equipe" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{C1864A1B-0B0A-44F9-B25C-3DC00BB84A6F}" name="Sexo" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{03C86AB8-DAC9-4C9A-88A4-2D5011F0A58E}" name="Idade" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{8337357E-563A-46C2-82BF-3B1B0568E153}" name="Nascimento" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{9887A2BA-74FB-434A-8771-38516E4F774F}" name="CPF" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{F4433FC6-D4E6-4D1F-98D4-77E7D1A887BA}" name="Nome" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{D5A6E3E8-91CB-4D68-9A74-D97F4D65094A}" name="Equipe" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{C1864A1B-0B0A-44F9-B25C-3DC00BB84A6F}" name="Sexo" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{03C86AB8-DAC9-4C9A-88A4-2D5011F0A58E}" name="Idade" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{8337357E-563A-46C2-82BF-3B1B0568E153}" name="Nascimento" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{9887A2BA-74FB-434A-8771-38516E4F774F}" name="CPF" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4EE7453-63EA-4448-B8B0-D17A4A1588D7}" name="Tabela2" displayName="Tabela2" ref="H1:H7" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4EE7453-63EA-4448-B8B0-D17A4A1588D7}" name="Tabela2" displayName="Tabela2" ref="H1:H7" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="H1:H7" xr:uid="{F4EE7453-63EA-4448-B8B0-D17A4A1588D7}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{541B7CCB-95A5-44E5-87FB-217BCA09DD48}" name="Equipe" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{541B7CCB-95A5-44E5-87FB-217BCA09DD48}" name="Equipe" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1241,8 +1331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D11AF4-2C8D-4548-9F11-4E03C4C35DE5}">
   <dimension ref="A1:H7089"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1280,7 +1370,7 @@
         <v>67</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>69</v>
@@ -1314,7 +1404,7 @@
       <c r="E3" s="10"/>
       <c r="F3" s="11"/>
       <c r="H3" s="14" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1675,7 +1765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4078EFF-B788-452D-9850-73BA89964DF3}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1720,4 +1810,231 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2D9D42-156D-4DF7-A051-A2119A9FC5DA}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="17">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="18"/>
+      <c r="B2" s="19"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="20">
+        <v>44927</v>
+      </c>
+      <c r="B3" s="21">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="20">
+        <v>44958</v>
+      </c>
+      <c r="B4" s="21">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="20">
+        <v>44986</v>
+      </c>
+      <c r="B5" s="21">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="20">
+        <v>45017</v>
+      </c>
+      <c r="B6" s="21">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="20">
+        <v>45047</v>
+      </c>
+      <c r="B7" s="21">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="20">
+        <v>45078</v>
+      </c>
+      <c r="B8" s="21">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="20">
+        <v>45108</v>
+      </c>
+      <c r="B9" s="21">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="20">
+        <v>45139</v>
+      </c>
+      <c r="B10" s="21">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="20">
+        <v>45170</v>
+      </c>
+      <c r="B11" s="21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="20">
+        <v>45200</v>
+      </c>
+      <c r="B12" s="21">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="20">
+        <v>45231</v>
+      </c>
+      <c r="B13" s="21"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="20">
+        <v>45261</v>
+      </c>
+      <c r="B14" s="21"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" s="22">
+        <f>SUM(B3:B14)</f>
+        <v>69202</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B14" xr:uid="{B48FF9EB-AE1C-438B-AC1F-0DB994A12E90}">
+      <formula1>SUM($B$3:$B$14)&lt;=$B$1</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D24952-8A5E-4EE6-9632-C79ADECF1955}">
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A3:A14 A2" xr:uid="{0293E7A7-DBFB-4427-A098-22AE7F208A5F}">
+      <formula1>COUNTIFS(A:A,A1)&lt;2</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>